<commit_message>
Modif index et descrfiption SDOBundle 90cfa8821d0abe41c44cf6022f19aeed2f9d199e
</commit_message>
<xml_diff>
--- a/180-rc-synthèse-des-ressources/ig/StructureDefinition-sdo-bundle-resultat-recherche-notification-esms.xlsx
+++ b/180-rc-synthèse-des-ressources/ig/StructureDefinition-sdo-bundle-resultat-recherche-notification-esms.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-30T12:00:20+00:00</t>
+    <t>2024-10-01T07:24:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil SDO pour la définition du Bundle de réponse à la recherche d'une notification</t>
+    <t>Profil ESMS-SDO pour la définition du Bundle de réponse à la recherche d'une notification</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>